<commit_message>
Nombre de usuario en navbar
</commit_message>
<xml_diff>
--- a/listaAlumnosTcontrol2020.xlsx
+++ b/listaAlumnosTcontrol2020.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DayClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724AD02E-600D-4106-9A81-6DA777B1D84D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2406EE3F-3DF0-41A8-BE58-8F40E3E9340E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CD408EB4-068D-41B0-997F-ECDE1FC04684}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{CD408EB4-068D-41B0-997F-ECDE1FC04684}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>dni</t>
   </si>
@@ -54,112 +54,88 @@
     <t>Ainsley</t>
   </si>
   <si>
-    <t>Cano</t>
-  </si>
-  <si>
-    <t>Rosa Maria</t>
-  </si>
-  <si>
-    <t>Cantu</t>
-  </si>
-  <si>
-    <t>Gabriel</t>
-  </si>
-  <si>
-    <t>Carr</t>
-  </si>
-  <si>
-    <t>Fay</t>
-  </si>
-  <si>
-    <t>Carson</t>
-  </si>
-  <si>
-    <t>Brian</t>
-  </si>
-  <si>
-    <t>Carver</t>
-  </si>
-  <si>
-    <t>Clinton</t>
-  </si>
-  <si>
-    <t>Case</t>
-  </si>
-  <si>
-    <t>Barrett</t>
-  </si>
-  <si>
-    <t>Haney</t>
-  </si>
-  <si>
-    <t>Jarrod</t>
-  </si>
-  <si>
-    <t>Hansen</t>
-  </si>
-  <si>
-    <t>Timon</t>
-  </si>
-  <si>
-    <t>Harris</t>
-  </si>
-  <si>
     <t>Cameron</t>
   </si>
   <si>
-    <t>Hartman</t>
-  </si>
-  <si>
-    <t>Zahir</t>
-  </si>
-  <si>
-    <t>Henderson</t>
-  </si>
-  <si>
     <t>Finn</t>
   </si>
   <si>
-    <t>Herman</t>
-  </si>
-  <si>
-    <t>Eve</t>
-  </si>
-  <si>
-    <t>Murphy</t>
-  </si>
-  <si>
-    <t>Ayanna</t>
-  </si>
-  <si>
-    <t>Demetrius</t>
-  </si>
-  <si>
-    <t>Nelson</t>
-  </si>
-  <si>
-    <t>Germane</t>
-  </si>
-  <si>
-    <t>Newton</t>
-  </si>
-  <si>
-    <t>Timothy</t>
-  </si>
-  <si>
-    <t>Nielsen</t>
-  </si>
-  <si>
-    <t>Pascale</t>
-  </si>
-  <si>
-    <t>Dias</t>
-  </si>
-  <si>
-    <t>Pedro</t>
-  </si>
-  <si>
-    <t>Meses</t>
+    <t>Aguirre</t>
+  </si>
+  <si>
+    <t>Imelda</t>
+  </si>
+  <si>
+    <t>Alfaro</t>
+  </si>
+  <si>
+    <t>Cristina</t>
+  </si>
+  <si>
+    <t>Allison</t>
+  </si>
+  <si>
+    <t>Alvarado</t>
+  </si>
+  <si>
+    <t>Maite</t>
+  </si>
+  <si>
+    <t>Andrada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pamela </t>
+  </si>
+  <si>
+    <t>Antares</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Atkinson</t>
+  </si>
+  <si>
+    <t>Libby</t>
+  </si>
+  <si>
+    <t>Barker</t>
+  </si>
+  <si>
+    <t>Nissim</t>
+  </si>
+  <si>
+    <t>Barry</t>
+  </si>
+  <si>
+    <t>Beard</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Beasley</t>
+  </si>
+  <si>
+    <t>Aimee</t>
+  </si>
+  <si>
+    <t>Benton</t>
+  </si>
+  <si>
+    <t>Abel</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Perex</t>
+  </si>
+  <si>
+    <t>Mayra</t>
+  </si>
+  <si>
+    <t>García</t>
   </si>
 </sst>
 </file>
@@ -539,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86421EA8-BD1F-4D4E-B554-7B0D03F06301}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,178 +537,178 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42906639</v>
+        <v>48637507</v>
       </c>
       <c r="B2" s="1">
-        <v>59479</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>41096</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41989681</v>
+        <v>46586634</v>
       </c>
       <c r="B3" s="1">
-        <v>73003</v>
+        <v>41050</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>30388106</v>
+        <v>9190607</v>
       </c>
       <c r="B4" s="1">
-        <v>51868</v>
+        <v>41030</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>27374218</v>
+        <v>44685116</v>
       </c>
       <c r="B5" s="1">
-        <v>58752</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>41146</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>31636157</v>
+        <v>18147102</v>
       </c>
       <c r="B6" s="1">
-        <v>81679</v>
+        <v>41173</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>49953301</v>
+        <v>43677391</v>
       </c>
       <c r="B7" s="1">
-        <v>61584</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>41093</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>29117970</v>
+        <v>12004396</v>
       </c>
       <c r="B8" s="1">
-        <v>83577</v>
+        <v>41136</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45266483</v>
+        <v>7366016</v>
       </c>
       <c r="B9" s="1">
-        <v>69932</v>
+        <v>41163</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>21409081</v>
+        <v>42906639</v>
       </c>
       <c r="B10" s="1">
-        <v>44683</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>41167</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>18780604</v>
+        <v>30388106</v>
       </c>
       <c r="B11" s="1">
-        <v>52979</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>41003</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>49867796</v>
+        <v>41989681</v>
       </c>
       <c r="B12" s="1">
-        <v>80480</v>
+        <v>41069</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>7029267</v>
+        <v>24682669</v>
       </c>
       <c r="B13" s="1">
-        <v>88033</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="1" t="s">
+        <v>41073</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>14669989</v>
+        <v>22330635</v>
       </c>
       <c r="B14" s="1">
-        <v>60823</v>
+        <v>41100</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>27</v>
@@ -743,38 +719,38 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>15307164</v>
+        <v>15427371</v>
       </c>
       <c r="B15" s="1">
-        <v>82923</v>
-      </c>
-      <c r="C15" s="2" t="s">
+        <v>41002</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>9478391</v>
+        <v>22621912</v>
       </c>
       <c r="B16" s="1">
-        <v>89861</v>
-      </c>
-      <c r="C16" s="2" t="s">
+        <v>41000</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>24556744</v>
+        <v>111</v>
       </c>
       <c r="B17" s="1">
-        <v>47299</v>
+        <v>222</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>33</v>
@@ -785,87 +761,47 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>10507943</v>
+        <v>123</v>
       </c>
       <c r="B18" s="1">
-        <v>80383</v>
+        <v>456</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>45757180</v>
-      </c>
-      <c r="B19" s="1">
-        <v>87563</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>31400914</v>
-      </c>
-      <c r="B20" s="1">
-        <v>45399</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>18843297</v>
-      </c>
-      <c r="B21" s="1">
-        <v>63387</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>111111</v>
-      </c>
-      <c r="B22" s="3">
-        <v>1111111</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>22222</v>
-      </c>
-      <c r="B23" s="3">
-        <v>222222</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>